<commit_message>
20.06.13 dynamic snake tail color
</commit_message>
<xml_diff>
--- a/회원관리(테스트용).xlsx
+++ b/회원관리(테스트용).xlsx
@@ -361,7 +361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C246"/>
+  <dimension ref="A1:C253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -2869,6 +2869,76 @@
         <v>245</v>
       </c>
     </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>-85</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>종합설계</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>3550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>